<commit_message>
Column width adjusted for Payment sheet
</commit_message>
<xml_diff>
--- a/section2/DhanaBhuma_Week2Homework .xlsx
+++ b/section2/DhanaBhuma_Week2Homework .xlsx
@@ -702,7 +702,7 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -710,7 +710,22 @@
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="28">
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment wrapText="1"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -962,9 +977,6 @@
       <alignment vertical="center"/>
     </dxf>
     <dxf>
-      <alignment wrapText="1"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     </dxf>
     <dxf>
@@ -1001,7 +1013,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1085,7 +1096,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1262,11 +1272,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="191126912"/>
-        <c:axId val="191149184"/>
+        <c:axId val="191501824"/>
+        <c:axId val="191503360"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="191126912"/>
+        <c:axId val="191501824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1275,7 +1285,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191149184"/>
+        <c:crossAx val="191503360"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1283,7 +1293,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191149184"/>
+        <c:axId val="191503360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1294,14 +1304,13 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191126912"/>
+        <c:crossAx val="191501824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1441,11 +1450,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="191063168"/>
-        <c:axId val="191064704"/>
+        <c:axId val="191523840"/>
+        <c:axId val="191714048"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="191063168"/>
+        <c:axId val="191523840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1454,7 +1463,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191064704"/>
+        <c:crossAx val="191714048"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1462,7 +1471,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="191064704"/>
+        <c:axId val="191714048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1473,7 +1482,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="191063168"/>
+        <c:crossAx val="191523840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4455,17 +4464,17 @@
   <dataFields count="1">
     <dataField name="Sum of Tax Inclusive Amount" fld="4" baseField="6" baseItem="1" numFmtId="164"/>
   </dataFields>
-  <formats count="11">
-    <format dxfId="23">
+  <formats count="13">
+    <format dxfId="27">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="22">
+    <format dxfId="26">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="21">
+    <format dxfId="25">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0"/>
     </format>
-    <format dxfId="20">
+    <format dxfId="24">
       <pivotArea outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -4474,26 +4483,32 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="19">
+    <format dxfId="23">
+      <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
+    </format>
+    <format dxfId="22">
+      <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
+    </format>
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="18">
+    <format dxfId="20">
       <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="17">
+    <format dxfId="19">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="16">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
-    <format dxfId="15">
+    <format dxfId="3">
+      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
+    </format>
+    <format dxfId="1">
       <pivotArea field="8" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="14">
+    <format dxfId="0">
       <pivotArea field="6" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
-    </format>
-    <format dxfId="13">
-      <pivotArea dataOnly="0" labelOnly="1" outline="0" axis="axisValues" fieldPosition="0"/>
     </format>
   </formats>
   <chartFormats count="4">
@@ -4555,18 +4570,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:I210" totalsRowShown="0" headerRowDxfId="12" dataDxfId="10" headerRowBorderDxfId="11" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:I210" totalsRowShown="0" headerRowDxfId="17" dataDxfId="15" headerRowBorderDxfId="16" tableBorderDxfId="14">
   <autoFilter ref="A2:I210"/>
   <tableColumns count="9">
-    <tableColumn id="1" name="Document Date" dataDxfId="8"/>
-    <tableColumn id="2" name="Supplier" dataDxfId="7"/>
-    <tableColumn id="3" name="Reference" dataDxfId="6"/>
-    <tableColumn id="4" name="Description" dataDxfId="5"/>
-    <tableColumn id="5" name="Tax Inclusive Amount" dataDxfId="4" dataCellStyle="Comma"/>
-    <tableColumn id="6" name="Tax Code" dataDxfId="3"/>
-    <tableColumn id="7" name="Bank Code" dataDxfId="2"/>
-    <tableColumn id="8" name="Account Code" dataDxfId="1"/>
-    <tableColumn id="9" name="Payment Date" dataDxfId="0"/>
+    <tableColumn id="1" name="Document Date" dataDxfId="13"/>
+    <tableColumn id="2" name="Supplier" dataDxfId="12"/>
+    <tableColumn id="3" name="Reference" dataDxfId="11"/>
+    <tableColumn id="4" name="Description" dataDxfId="10"/>
+    <tableColumn id="5" name="Tax Inclusive Amount" dataDxfId="9" dataCellStyle="Comma"/>
+    <tableColumn id="6" name="Tax Code" dataDxfId="8"/>
+    <tableColumn id="7" name="Bank Code" dataDxfId="7"/>
+    <tableColumn id="8" name="Account Code" dataDxfId="6"/>
+    <tableColumn id="9" name="Payment Date" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4861,7 +4876,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5351,15 +5366,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
-    <col min="3" max="3" width="22.7109375" customWidth="1"/>
+    <col min="1" max="3" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -5447,7 +5458,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>